<commit_message>
Bug fixes based on Vidhya's feedback
* 24-hour day is now used (instead of 12 hour day)
* User cannot execute writer node without configuring it first
* Better output file name validation (tells the user before execution, rather than inexplicably failing during execution)
* Dates previously could be accidently saved with invalid byte order
</commit_message>
<xml_diff>
--- a/eclipse-workspace/test-files/final-version-test-files/ManyDataTypes.xlsx
+++ b/eclipse-workspace/test-files/final-version-test-files/ManyDataTypes.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>36526</v>
+        <v>367</v>
       </c>
       <c r="D2" s="2">
         <v>4.943287037037037E-2</v>
@@ -470,10 +470,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>37289</v>
+        <v>764</v>
       </c>
       <c r="D3" s="2">
-        <v>9.886574074074074E-2</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="E3" s="1">
         <v>22074.583333333332</v>
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>43893</v>
+        <v>37683</v>
       </c>
       <c r="D4" s="2">
         <v>0.14829861111111112</v>
@@ -526,7 +526,7 @@
         <v>36558</v>
       </c>
       <c r="D5" s="2">
-        <v>0.19773148148148148</v>
+        <v>0.78055555555555556</v>
       </c>
       <c r="E5" s="1">
         <v>22076.166666666668</v>
@@ -552,7 +552,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>18388</v>
+        <v>239360</v>
       </c>
       <c r="E6" s="1">
         <v>22077.208333333332</v>

</xml_diff>